<commit_message>
Merged PR 7547: PRI-19857 Export Campaign to Excel - Add ADUs to Contract Tab
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
@@ -228,7 +228,7 @@
     <t>3/24, 3/28</t>
   </si>
   <si>
-    <t xml:space="preserve">1Q '20 EF :30s </t>
+    <t>1Q '20 EF :30s</t>
   </si>
   <si>
     <t>3/16-17, 3/21</t>
@@ -249,7 +249,7 @@
     <t>1Q '20 EM :45s eq.</t>
   </si>
   <si>
-    <t xml:space="preserve">1Q '20 EM :30s </t>
+    <t>1Q '20 EM :30s</t>
   </si>
   <si>
     <t>1Q '20 EM Total</t>
@@ -258,7 +258,7 @@
     <t>1Q '20 MDN :45s eq.</t>
   </si>
   <si>
-    <t xml:space="preserve">1Q '20 MDN :30s </t>
+    <t>1Q '20 MDN :30s</t>
   </si>
   <si>
     <t>1Q '20 MDN Total</t>
@@ -285,7 +285,7 @@
     <t>4/7, 4/9-11</t>
   </si>
   <si>
-    <t xml:space="preserve">2Q '20 EF :30s </t>
+    <t>2Q '20 EF :30s</t>
   </si>
   <si>
     <t>4/8-10</t>
@@ -300,7 +300,7 @@
     <t>2Q '20 EM :45s eq.</t>
   </si>
   <si>
-    <t xml:space="preserve">2Q '20 EM :30s </t>
+    <t>2Q '20 EM :30s</t>
   </si>
   <si>
     <t>2Q '20 EM Total</t>
@@ -309,7 +309,7 @@
     <t>2Q '20 MDN :45s eq.</t>
   </si>
   <si>
-    <t xml:space="preserve">2Q '20 MDN :30s </t>
+    <t>2Q '20 MDN :30s</t>
   </si>
   <si>
     <t>2Q '20 MDN Total</t>
@@ -354,10 +354,13 @@
     <t>3/9/2020</t>
   </si>
   <si>
-    <t>:45s eq.</t>
+    <t>:30s</t>
   </si>
   <si>
     <t>Even</t>
+  </si>
+  <si>
+    <t>:45s eq.</t>
   </si>
   <si>
     <t>EM</t>
@@ -372,10 +375,10 @@
     <t>3/23/2020</t>
   </si>
   <si>
-    <t>:30s</t>
+    <t>1Q '20 Totals</t>
   </si>
   <si>
-    <t>1Q '20 Totals</t>
+    <t>45 eq.</t>
   </si>
   <si>
     <t>Q2 2020</t>
@@ -836,9 +839,6 @@
   </si>
   <si>
     <t>Length</t>
-  </si>
-  <si>
-    <t>45 eq.</t>
   </si>
   <si>
     <t>30</t>
@@ -2458,7 +2458,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:T60"/>
+  <dimension ref="A2:T73"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0" tabSelected="1">
       <selection activeCell="C5" sqref="C5"/>
@@ -2652,13 +2652,13 @@
         <v>0</v>
       </c>
       <c r="H9" s="85">
-        <v>40000</v>
+        <v>400</v>
       </c>
       <c r="I9" s="83">
         <v>0</v>
       </c>
       <c r="J9" s="93">
-        <v>1600.0000000000002</v>
+        <v>16</v>
       </c>
       <c r="K9" s="95">
         <v>25</v>
@@ -2670,7 +2670,7 @@
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="81" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D10" s="82" t="s">
         <v>105</v>
@@ -2679,7 +2679,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="84" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G10" s="85">
         <v>0</v>
@@ -2718,13 +2718,13 @@
         <v>0</v>
       </c>
       <c r="H11" s="85">
-        <v>20000</v>
+        <v>99400</v>
       </c>
       <c r="I11" s="83">
         <v>0</v>
       </c>
       <c r="J11" s="93">
-        <v>800.00000000000011</v>
+        <v>3976.0000000000005</v>
       </c>
       <c r="K11" s="95">
         <v>25</v>
@@ -2736,16 +2736,16 @@
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="81" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D12" s="82" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E12" s="83">
         <v>0</v>
       </c>
       <c r="F12" s="84" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G12" s="85">
         <v>0</v>
@@ -2769,10 +2769,10 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="81" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D13" s="82" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E13" s="83">
         <v>0</v>
@@ -2784,13 +2784,13 @@
         <v>0</v>
       </c>
       <c r="H13" s="85">
-        <v>40000</v>
+        <v>200</v>
       </c>
       <c r="I13" s="83">
         <v>0</v>
       </c>
       <c r="J13" s="93">
-        <v>1600.0000000000002</v>
+        <v>8</v>
       </c>
       <c r="K13" s="95">
         <v>25</v>
@@ -2802,16 +2802,16 @@
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="81" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D14" s="82" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E14" s="83">
         <v>0</v>
       </c>
       <c r="F14" s="84" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G14" s="85">
         <v>0</v>
@@ -2850,13 +2850,13 @@
         <v>0</v>
       </c>
       <c r="H15" s="85">
-        <v>40000</v>
+        <v>400</v>
       </c>
       <c r="I15" s="83">
         <v>0</v>
       </c>
       <c r="J15" s="93">
-        <v>1600.0000000000002</v>
+        <v>16</v>
       </c>
       <c r="K15" s="95">
         <v>25</v>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="81" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D16" s="82" t="s">
         <v>111</v>
@@ -2877,7 +2877,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="84" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G16" s="85">
         <v>0</v>
@@ -2916,13 +2916,13 @@
         <v>0</v>
       </c>
       <c r="H17" s="85">
-        <v>20000</v>
+        <v>99400</v>
       </c>
       <c r="I17" s="83">
         <v>0</v>
       </c>
       <c r="J17" s="93">
-        <v>800.00000000000011</v>
+        <v>3976.0000000000005</v>
       </c>
       <c r="K17" s="95">
         <v>25</v>
@@ -2937,25 +2937,25 @@
         <v>109</v>
       </c>
       <c r="D18" s="82" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E18" s="83">
         <v>0</v>
       </c>
       <c r="F18" s="84" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G18" s="85">
         <v>0</v>
       </c>
       <c r="H18" s="85">
-        <v>200</v>
+        <v>40000</v>
       </c>
       <c r="I18" s="83">
         <v>0</v>
       </c>
       <c r="J18" s="93">
-        <v>8</v>
+        <v>1600.0000000000002</v>
       </c>
       <c r="K18" s="95">
         <v>25</v>
@@ -2967,28 +2967,28 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="81" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D19" s="82" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E19" s="83">
         <v>0</v>
       </c>
       <c r="F19" s="84" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G19" s="85">
         <v>0</v>
       </c>
       <c r="H19" s="85">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="I19" s="83">
         <v>0</v>
       </c>
       <c r="J19" s="93">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K19" s="95">
         <v>25</v>
@@ -3000,28 +3000,28 @@
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="81" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="83">
+        <v>0</v>
+      </c>
+      <c r="F20" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="82" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="83">
-        <v>0</v>
-      </c>
-      <c r="F20" s="84" t="s">
-        <v>112</v>
-      </c>
       <c r="G20" s="85">
         <v>0</v>
       </c>
       <c r="H20" s="85">
-        <v>99400</v>
+        <v>20000</v>
       </c>
       <c r="I20" s="83">
         <v>0</v>
       </c>
       <c r="J20" s="93">
-        <v>3976.0000000000005</v>
+        <v>800.00000000000011</v>
       </c>
       <c r="K20" s="95">
         <v>25</v>
@@ -3033,28 +3033,28 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="81" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D21" s="82" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E21" s="83">
         <v>0</v>
       </c>
       <c r="F21" s="84" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G21" s="85">
         <v>0</v>
       </c>
       <c r="H21" s="85">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="I21" s="83">
         <v>0</v>
       </c>
       <c r="J21" s="93">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K21" s="95">
         <v>25</v>
@@ -3069,25 +3069,25 @@
         <v>104</v>
       </c>
       <c r="D22" s="82" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E22" s="83">
         <v>0</v>
       </c>
       <c r="F22" s="84" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G22" s="85">
         <v>0</v>
       </c>
       <c r="H22" s="85">
-        <v>400</v>
+        <v>40000</v>
       </c>
       <c r="I22" s="83">
         <v>0</v>
       </c>
       <c r="J22" s="93">
-        <v>16</v>
+        <v>1600.0000000000002</v>
       </c>
       <c r="K22" s="95">
         <v>25</v>
@@ -3099,16 +3099,16 @@
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="81" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D23" s="82" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E23" s="83">
         <v>0</v>
       </c>
       <c r="F23" s="84" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G23" s="85">
         <v>0</v>
@@ -3135,25 +3135,25 @@
         <v>109</v>
       </c>
       <c r="D24" s="82" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E24" s="83">
         <v>0</v>
       </c>
       <c r="F24" s="84" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G24" s="85">
         <v>0</v>
       </c>
       <c r="H24" s="85">
-        <v>200</v>
+        <v>40000</v>
       </c>
       <c r="I24" s="83">
         <v>0</v>
       </c>
       <c r="J24" s="93">
-        <v>8</v>
+        <v>1600.0000000000002</v>
       </c>
       <c r="K24" s="95">
         <v>25</v>
@@ -3165,28 +3165,28 @@
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="81" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D25" s="82" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E25" s="83">
         <v>0</v>
       </c>
       <c r="F25" s="84" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G25" s="85">
         <v>0</v>
       </c>
       <c r="H25" s="85">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="I25" s="83">
         <v>0</v>
       </c>
       <c r="J25" s="93">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K25" s="95">
         <v>25</v>
@@ -3198,38 +3198,34 @@
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="81" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="83">
+        <v>0</v>
+      </c>
+      <c r="F26" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="D26" s="82" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="83">
-        <v>0</v>
-      </c>
-      <c r="F26" s="84" t="s">
-        <v>112</v>
-      </c>
       <c r="G26" s="85">
         <v>0</v>
       </c>
       <c r="H26" s="85">
-        <v>99400</v>
+        <v>20000</v>
       </c>
       <c r="I26" s="83">
         <v>0</v>
       </c>
       <c r="J26" s="93">
-        <v>3976.0000000000005</v>
+        <v>800.00000000000011</v>
       </c>
       <c r="K26" s="95">
         <v>25</v>
       </c>
     </row>
     <row r="27" ht="24" customHeight="1">
-      <c r="A27" s="99" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" s="4"/>
       <c r="C27" s="39"/>
       <c r="D27" s="91" t="s">
         <v>113</v>
@@ -3258,7 +3254,7 @@
     </row>
     <row r="29">
       <c r="C29" s="53" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="H29" s="30"/>
       <c r="I29" s="30"/>
@@ -3319,32 +3315,30 @@
         <v>103</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="81" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" s="82" t="s">
-        <v>115</v>
+      <c r="C31" s="81"/>
+      <c r="D31" s="82">
+        <v>43899</v>
       </c>
       <c r="E31" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="84" t="s">
-        <v>106</v>
-      </c>
-      <c r="G31" s="85">
-        <v>0</v>
-      </c>
-      <c r="H31" s="85">
-        <v>40000</v>
-      </c>
-      <c r="I31" s="83">
-        <v>0</v>
-      </c>
-      <c r="J31" s="93">
-        <v>1600.0000000000002</v>
-      </c>
-      <c r="K31" s="95">
-        <v>25</v>
+        <v>114</v>
+      </c>
+      <c r="G31" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="I31" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="J31" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="K31" s="95" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="32" ht="24" customHeight="1">
@@ -3352,32 +3346,30 @@
         <v>107</v>
       </c>
       <c r="B32" s="4"/>
-      <c r="C32" s="81" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" s="82" t="s">
-        <v>115</v>
+      <c r="C32" s="81"/>
+      <c r="D32" s="82">
+        <v>43906</v>
       </c>
       <c r="E32" s="83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="84" t="s">
-        <v>106</v>
-      </c>
-      <c r="G32" s="85">
-        <v>0</v>
-      </c>
-      <c r="H32" s="85">
-        <v>40000</v>
-      </c>
-      <c r="I32" s="83">
-        <v>0</v>
-      </c>
-      <c r="J32" s="93">
-        <v>1600.0000000000002</v>
-      </c>
-      <c r="K32" s="95">
-        <v>25</v>
+        <v>114</v>
+      </c>
+      <c r="G32" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="I32" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="J32" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="K32" s="95" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="33" ht="24" customHeight="1">
@@ -3385,182 +3377,133 @@
         <v>103</v>
       </c>
       <c r="B33" s="4"/>
-      <c r="C33" s="81" t="s">
-        <v>109</v>
-      </c>
-      <c r="D33" s="82" t="s">
+      <c r="C33" s="81"/>
+      <c r="D33" s="82">
+        <v>43913</v>
+      </c>
+      <c r="E33" s="83">
+        <v>1</v>
+      </c>
+      <c r="F33" s="84" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="I33" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="J33" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="K33" s="95" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" ht="24" customHeight="1">
+      <c r="C34" s="39"/>
+      <c r="D34" s="91" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="97">
+        <v>3</v>
+      </c>
+      <c r="F34" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="96" t="s">
+        <v>38</v>
+      </c>
+      <c r="H34" s="89" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="J34" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="K34" s="98" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="C36" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="E33" s="83">
-        <v>0</v>
-      </c>
-      <c r="F33" s="84" t="s">
-        <v>106</v>
-      </c>
-      <c r="G33" s="85">
-        <v>0</v>
-      </c>
-      <c r="H33" s="85">
-        <v>20000</v>
-      </c>
-      <c r="I33" s="83">
-        <v>0</v>
-      </c>
-      <c r="J33" s="93">
-        <v>800.00000000000011</v>
-      </c>
-      <c r="K33" s="95">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" ht="24" customHeight="1">
-      <c r="A34" s="99" t="s">
-        <v>107</v>
-      </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="81" t="s">
-        <v>104</v>
-      </c>
-      <c r="D34" s="82" t="s">
-        <v>116</v>
-      </c>
-      <c r="E34" s="83">
-        <v>0</v>
-      </c>
-      <c r="F34" s="84" t="s">
-        <v>106</v>
-      </c>
-      <c r="G34" s="85">
-        <v>0</v>
-      </c>
-      <c r="H34" s="85">
-        <v>40000</v>
-      </c>
-      <c r="I34" s="83">
-        <v>0</v>
-      </c>
-      <c r="J34" s="93">
-        <v>1600.0000000000002</v>
-      </c>
-      <c r="K34" s="95">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" ht="24" customHeight="1">
-      <c r="A35" s="99" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="81" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="82" t="s">
-        <v>116</v>
-      </c>
-      <c r="E35" s="83">
-        <v>0</v>
-      </c>
-      <c r="F35" s="84" t="s">
-        <v>106</v>
-      </c>
-      <c r="G35" s="85">
-        <v>0</v>
-      </c>
-      <c r="H35" s="85">
-        <v>40000</v>
-      </c>
-      <c r="I35" s="83">
-        <v>0</v>
-      </c>
-      <c r="J35" s="93">
-        <v>1600.0000000000002</v>
-      </c>
-      <c r="K35" s="95">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" ht="24" customHeight="1">
-      <c r="A36" s="99" t="s">
-        <v>107</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="81" t="s">
-        <v>109</v>
-      </c>
-      <c r="D36" s="82" t="s">
-        <v>116</v>
-      </c>
-      <c r="E36" s="83">
-        <v>0</v>
-      </c>
-      <c r="F36" s="84" t="s">
-        <v>106</v>
-      </c>
-      <c r="G36" s="85">
-        <v>0</v>
-      </c>
-      <c r="H36" s="85">
-        <v>20000</v>
-      </c>
-      <c r="I36" s="83">
-        <v>0</v>
-      </c>
-      <c r="J36" s="93">
-        <v>800.00000000000011</v>
-      </c>
-      <c r="K36" s="95">
-        <v>25</v>
-      </c>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="60"/>
+      <c r="T36" s="60"/>
     </row>
     <row r="37" ht="24" customHeight="1">
       <c r="A37" s="99" t="s">
-        <v>103</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="81" t="s">
-        <v>109</v>
-      </c>
-      <c r="D37" s="82" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" s="83">
-        <v>0</v>
-      </c>
-      <c r="F37" s="84" t="s">
-        <v>112</v>
-      </c>
-      <c r="G37" s="85">
-        <v>0</v>
-      </c>
-      <c r="H37" s="85">
-        <v>200</v>
-      </c>
-      <c r="I37" s="83">
-        <v>0</v>
-      </c>
-      <c r="J37" s="93">
-        <v>8</v>
-      </c>
-      <c r="K37" s="95">
+        <v>97</v>
+      </c>
+      <c r="C37" s="86" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="87" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="87" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="H37" s="87" t="s">
         <v>25</v>
       </c>
+      <c r="I37" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="J37" s="92" t="s">
+        <v>102</v>
+      </c>
+      <c r="K37" s="88" t="s">
+        <v>30</v>
+      </c>
+      <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="60"/>
+      <c r="S37" s="60"/>
+      <c r="T37" s="60"/>
     </row>
     <row r="38" ht="24" customHeight="1">
       <c r="A38" s="99" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="81" t="s">
         <v>104</v>
       </c>
       <c r="D38" s="82" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E38" s="83">
         <v>0</v>
       </c>
       <c r="F38" s="84" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G38" s="85">
         <v>0</v>
@@ -3580,32 +3523,32 @@
     </row>
     <row r="39" ht="24" customHeight="1">
       <c r="A39" s="99" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" s="83">
+        <v>0</v>
+      </c>
+      <c r="F39" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="82" t="s">
-        <v>115</v>
-      </c>
-      <c r="E39" s="83">
-        <v>0</v>
-      </c>
-      <c r="F39" s="84" t="s">
-        <v>112</v>
-      </c>
       <c r="G39" s="85">
         <v>0</v>
       </c>
       <c r="H39" s="85">
-        <v>99400</v>
+        <v>40000</v>
       </c>
       <c r="I39" s="83">
         <v>0</v>
       </c>
       <c r="J39" s="93">
-        <v>3976.0000000000005</v>
+        <v>1600.0000000000002</v>
       </c>
       <c r="K39" s="95">
         <v>25</v>
@@ -3613,7 +3556,7 @@
     </row>
     <row r="40" ht="24" customHeight="1">
       <c r="A40" s="99" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="81" t="s">
@@ -3626,19 +3569,19 @@
         <v>0</v>
       </c>
       <c r="F40" s="84" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G40" s="85">
         <v>0</v>
       </c>
       <c r="H40" s="85">
-        <v>200</v>
+        <v>99400</v>
       </c>
       <c r="I40" s="83">
         <v>0</v>
       </c>
       <c r="J40" s="93">
-        <v>8</v>
+        <v>3976.0000000000005</v>
       </c>
       <c r="K40" s="95">
         <v>25</v>
@@ -3646,11 +3589,11 @@
     </row>
     <row r="41" ht="24" customHeight="1">
       <c r="A41" s="99" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="81" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D41" s="82" t="s">
         <v>116</v>
@@ -3659,19 +3602,19 @@
         <v>0</v>
       </c>
       <c r="F41" s="84" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G41" s="85">
         <v>0</v>
       </c>
       <c r="H41" s="85">
-        <v>400</v>
+        <v>40000</v>
       </c>
       <c r="I41" s="83">
         <v>0</v>
       </c>
       <c r="J41" s="93">
-        <v>16</v>
+        <v>1600.0000000000002</v>
       </c>
       <c r="K41" s="95">
         <v>25</v>
@@ -3679,11 +3622,11 @@
     </row>
     <row r="42" ht="24" customHeight="1">
       <c r="A42" s="99" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="81" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D42" s="82" t="s">
         <v>116</v>
@@ -3692,19 +3635,19 @@
         <v>0</v>
       </c>
       <c r="F42" s="84" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G42" s="85">
         <v>0</v>
       </c>
       <c r="H42" s="85">
-        <v>99400</v>
+        <v>200</v>
       </c>
       <c r="I42" s="83">
         <v>0</v>
       </c>
       <c r="J42" s="93">
-        <v>3976.0000000000005</v>
+        <v>8</v>
       </c>
       <c r="K42" s="95">
         <v>25</v>
@@ -3712,309 +3655,683 @@
     </row>
     <row r="43" ht="24" customHeight="1">
       <c r="A43" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="81" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" s="83">
+        <v>0</v>
+      </c>
+      <c r="F43" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="G43" s="85">
+        <v>0</v>
+      </c>
+      <c r="H43" s="85">
+        <v>20000</v>
+      </c>
+      <c r="I43" s="83">
+        <v>0</v>
+      </c>
+      <c r="J43" s="93">
+        <v>800.00000000000011</v>
+      </c>
+      <c r="K43" s="95">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" ht="24" customHeight="1">
+      <c r="A44" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="91" t="s">
+      <c r="B44" s="4"/>
+      <c r="C44" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="82" t="s">
         <v>117</v>
       </c>
-      <c r="E43" s="97">
-        <v>0</v>
-      </c>
-      <c r="F43" s="90" t="s">
+      <c r="E44" s="83">
+        <v>0</v>
+      </c>
+      <c r="F44" s="84" t="s">
+        <v>106</v>
+      </c>
+      <c r="G44" s="85">
+        <v>0</v>
+      </c>
+      <c r="H44" s="85">
+        <v>400</v>
+      </c>
+      <c r="I44" s="83">
+        <v>0</v>
+      </c>
+      <c r="J44" s="93">
+        <v>16</v>
+      </c>
+      <c r="K44" s="95">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" ht="24" customHeight="1">
+      <c r="A45" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="E45" s="83">
+        <v>0</v>
+      </c>
+      <c r="F45" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="G45" s="85">
+        <v>0</v>
+      </c>
+      <c r="H45" s="85">
+        <v>40000</v>
+      </c>
+      <c r="I45" s="83">
+        <v>0</v>
+      </c>
+      <c r="J45" s="93">
+        <v>1600.0000000000002</v>
+      </c>
+      <c r="K45" s="95">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" ht="24" customHeight="1">
+      <c r="A46" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" s="83">
+        <v>0</v>
+      </c>
+      <c r="F46" s="84" t="s">
+        <v>106</v>
+      </c>
+      <c r="G46" s="85">
+        <v>0</v>
+      </c>
+      <c r="H46" s="85">
+        <v>99400</v>
+      </c>
+      <c r="I46" s="83">
+        <v>0</v>
+      </c>
+      <c r="J46" s="93">
+        <v>3976.0000000000005</v>
+      </c>
+      <c r="K46" s="95">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" ht="24" customHeight="1">
+      <c r="A47" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="E47" s="83">
+        <v>0</v>
+      </c>
+      <c r="F47" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="G47" s="85">
+        <v>0</v>
+      </c>
+      <c r="H47" s="85">
+        <v>40000</v>
+      </c>
+      <c r="I47" s="83">
+        <v>0</v>
+      </c>
+      <c r="J47" s="93">
+        <v>1600.0000000000002</v>
+      </c>
+      <c r="K47" s="95">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" ht="24" customHeight="1">
+      <c r="A48" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="81" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="E48" s="83">
+        <v>0</v>
+      </c>
+      <c r="F48" s="84" t="s">
+        <v>106</v>
+      </c>
+      <c r="G48" s="85">
+        <v>0</v>
+      </c>
+      <c r="H48" s="85">
+        <v>200</v>
+      </c>
+      <c r="I48" s="83">
+        <v>0</v>
+      </c>
+      <c r="J48" s="93">
+        <v>8</v>
+      </c>
+      <c r="K48" s="95">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" ht="24" customHeight="1">
+      <c r="A49" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="81" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="82" t="s">
+        <v>117</v>
+      </c>
+      <c r="E49" s="83">
+        <v>0</v>
+      </c>
+      <c r="F49" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="G49" s="85">
+        <v>0</v>
+      </c>
+      <c r="H49" s="85">
+        <v>20000</v>
+      </c>
+      <c r="I49" s="83">
+        <v>0</v>
+      </c>
+      <c r="J49" s="93">
+        <v>800.00000000000011</v>
+      </c>
+      <c r="K49" s="95">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" ht="24" customHeight="1">
+      <c r="C50" s="39"/>
+      <c r="D50" s="91" t="s">
+        <v>118</v>
+      </c>
+      <c r="E50" s="97">
+        <v>0</v>
+      </c>
+      <c r="F50" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="G43" s="96" t="s">
+      <c r="G50" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="H43" s="89">
+      <c r="H50" s="89">
         <v>400000</v>
       </c>
-      <c r="I43" s="90" t="s">
+      <c r="I50" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="J43" s="94">
+      <c r="J50" s="94">
         <v>16000</v>
       </c>
-      <c r="K43" s="98">
+      <c r="K50" s="98">
         <v>25</v>
       </c>
     </row>
-    <row r="45" ht="24" customHeight="1">
-      <c r="C45" s="53" t="s">
+    <row r="52">
+      <c r="C52" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="H52" s="30"/>
+      <c r="I52" s="30"/>
+      <c r="J52" s="30"/>
+      <c r="K52" s="30"/>
+      <c r="L52" s="60"/>
+      <c r="M52" s="60"/>
+      <c r="N52" s="60"/>
+      <c r="O52" s="60"/>
+      <c r="P52" s="60"/>
+      <c r="Q52" s="60"/>
+      <c r="R52" s="60"/>
+      <c r="S52" s="60"/>
+      <c r="T52" s="60"/>
+    </row>
+    <row r="53" ht="24" customHeight="1">
+      <c r="A53" s="99" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="86" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="E53" s="87" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53" s="87" t="s">
+        <v>100</v>
+      </c>
+      <c r="G53" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="H53" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="I53" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="J53" s="92" t="s">
+        <v>102</v>
+      </c>
+      <c r="K53" s="88" t="s">
+        <v>30</v>
+      </c>
+      <c r="M53" s="60"/>
+      <c r="N53" s="60"/>
+      <c r="O53" s="60"/>
+      <c r="P53" s="60"/>
+      <c r="Q53" s="60"/>
+      <c r="R53" s="60"/>
+      <c r="S53" s="60"/>
+      <c r="T53" s="60"/>
+    </row>
+    <row r="54" ht="24" customHeight="1">
+      <c r="A54" s="99" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="82">
+        <v>43920</v>
+      </c>
+      <c r="E54" s="83">
+        <v>1</v>
+      </c>
+      <c r="F54" s="84" t="s">
+        <v>114</v>
+      </c>
+      <c r="G54" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="H54" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="I54" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="J54" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="K54" s="95" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" ht="24" customHeight="1">
+      <c r="A55" s="99" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="81"/>
+      <c r="D55" s="82">
+        <v>43927</v>
+      </c>
+      <c r="E55" s="83">
+        <v>1</v>
+      </c>
+      <c r="F55" s="84" t="s">
+        <v>114</v>
+      </c>
+      <c r="G55" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="H55" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="I55" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="J55" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="K55" s="95" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" ht="24" customHeight="1">
+      <c r="C56" s="39"/>
+      <c r="D56" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="I45" s="60"/>
-    </row>
-    <row r="46" ht="24" customHeight="1">
-      <c r="C46" s="100" t="s">
+      <c r="E56" s="97">
+        <v>2</v>
+      </c>
+      <c r="F56" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="G56" s="96" t="s">
+        <v>38</v>
+      </c>
+      <c r="H56" s="89" t="s">
+        <v>38</v>
+      </c>
+      <c r="I56" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="J56" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="K56" s="98" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" ht="24" customHeight="1">
+      <c r="C58" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="I58" s="60"/>
+    </row>
+    <row r="59" ht="24" customHeight="1">
+      <c r="C59" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="D46" s="101" t="s">
+      <c r="D59" s="101" t="s">
         <v>59</v>
       </c>
-      <c r="E46" s="101"/>
-      <c r="F46" s="101" t="s">
+      <c r="E59" s="101"/>
+      <c r="F59" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="G46" s="101"/>
-      <c r="H46" s="101" t="s">
+      <c r="G59" s="101"/>
+      <c r="H59" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="I46" s="102"/>
-    </row>
-    <row r="47" ht="24" customHeight="1">
-      <c r="C47" s="103">
-        <v>0</v>
-      </c>
-      <c r="D47" s="105">
+      <c r="I59" s="102"/>
+    </row>
+    <row r="60" ht="24" customHeight="1">
+      <c r="C60" s="103">
+        <v>0</v>
+      </c>
+      <c r="D60" s="105">
         <v>1000000</v>
       </c>
-      <c r="E47" s="105"/>
-      <c r="F47" s="104">
+      <c r="E60" s="105"/>
+      <c r="F60" s="104">
         <v>40000</v>
       </c>
-      <c r="G47" s="104"/>
-      <c r="H47" s="107">
+      <c r="G60" s="104"/>
+      <c r="H60" s="107">
         <v>25</v>
       </c>
-      <c r="I47" s="106"/>
-    </row>
-    <row r="48" ht="42.95" customHeight="1">
-      <c r="C48" s="110"/>
-      <c r="D48" s="111"/>
-      <c r="E48" s="111"/>
-      <c r="F48" s="112"/>
-      <c r="G48" s="112"/>
-      <c r="H48" s="108"/>
-      <c r="I48" s="108"/>
-    </row>
-    <row r="49" ht="24" customHeight="1">
-      <c r="C49" s="113" t="s">
-        <v>119</v>
-      </c>
-      <c r="D49" s="109"/>
-      <c r="E49" s="109"/>
-      <c r="F49" s="112"/>
-      <c r="G49" s="114" t="s">
+      <c r="I60" s="106"/>
+    </row>
+    <row r="61" ht="42.95" customHeight="1">
+      <c r="C61" s="110"/>
+      <c r="D61" s="111"/>
+      <c r="E61" s="111"/>
+      <c r="F61" s="112"/>
+      <c r="G61" s="112"/>
+      <c r="H61" s="108"/>
+      <c r="I61" s="108"/>
+    </row>
+    <row r="62" ht="24" customHeight="1">
+      <c r="C62" s="113" t="s">
         <v>120</v>
       </c>
-      <c r="H49" s="109"/>
-      <c r="I49" s="115"/>
-    </row>
-    <row r="50" ht="39.95" customHeight="1">
-      <c r="C50" s="110"/>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="112"/>
-      <c r="G50" s="112"/>
-      <c r="H50" s="108"/>
-      <c r="I50" s="108"/>
-    </row>
-    <row r="51" ht="48" customHeight="1" s="99" customFormat="1">
-      <c r="C51" s="55" t="s">
+      <c r="D62" s="109"/>
+      <c r="E62" s="109"/>
+      <c r="F62" s="112"/>
+      <c r="G62" s="114" t="s">
+        <v>121</v>
+      </c>
+      <c r="H62" s="109"/>
+      <c r="I62" s="115"/>
+    </row>
+    <row r="63" ht="39.95" customHeight="1">
+      <c r="C63" s="110"/>
+      <c r="D63" s="111"/>
+      <c r="E63" s="111"/>
+      <c r="F63" s="112"/>
+      <c r="G63" s="112"/>
+      <c r="H63" s="108"/>
+      <c r="I63" s="108"/>
+    </row>
+    <row r="64" ht="48" customHeight="1" s="99" customFormat="1">
+      <c r="C64" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="D51" s="136" t="str">
+      <c r="D64" s="136" t="str">
         <f>'PROPOSAL'!F37</f>
         <v>~80% Minimum TV HH Coverage | Blackout Markets: Lansing, Wilmington, Presque Isle | Preferential Markets: Philadelphia, Macon, New York, Binghamton</v>
       </c>
-      <c r="E51" s="136"/>
-      <c r="F51" s="136"/>
-      <c r="G51" s="136"/>
-      <c r="H51" s="136"/>
-      <c r="I51" s="136"/>
-      <c r="J51" s="136"/>
-      <c r="K51" s="136"/>
-      <c r="L51" s="126"/>
-      <c r="M51" s="126"/>
-      <c r="N51" s="126"/>
-      <c r="O51" s="126"/>
-      <c r="P51" s="126"/>
-      <c r="Q51" s="126"/>
-      <c r="R51" s="126"/>
-    </row>
-    <row r="52" ht="8.1" customHeight="1" s="99" customFormat="1">
-      <c r="C52" s="2"/>
-      <c r="D52" s="127"/>
-      <c r="E52" s="127"/>
-      <c r="F52" s="127"/>
-      <c r="G52" s="127"/>
-      <c r="H52" s="127"/>
-      <c r="I52" s="127"/>
-      <c r="J52" s="127"/>
-      <c r="K52" s="127"/>
-      <c r="L52" s="76"/>
-      <c r="M52" s="76"/>
-      <c r="N52" s="76"/>
-      <c r="O52" s="76"/>
-      <c r="P52" s="76"/>
-      <c r="Q52" s="76"/>
-      <c r="R52" s="76"/>
-    </row>
-    <row r="53" ht="48" customHeight="1" s="117" customFormat="1">
-      <c r="C53" s="55" t="s">
+      <c r="E64" s="136"/>
+      <c r="F64" s="136"/>
+      <c r="G64" s="136"/>
+      <c r="H64" s="136"/>
+      <c r="I64" s="136"/>
+      <c r="J64" s="136"/>
+      <c r="K64" s="136"/>
+      <c r="L64" s="126"/>
+      <c r="M64" s="126"/>
+      <c r="N64" s="126"/>
+      <c r="O64" s="126"/>
+      <c r="P64" s="126"/>
+      <c r="Q64" s="126"/>
+      <c r="R64" s="126"/>
+    </row>
+    <row r="65" ht="8.1" customHeight="1" s="99" customFormat="1">
+      <c r="C65" s="2"/>
+      <c r="D65" s="127"/>
+      <c r="E65" s="127"/>
+      <c r="F65" s="127"/>
+      <c r="G65" s="127"/>
+      <c r="H65" s="127"/>
+      <c r="I65" s="127"/>
+      <c r="J65" s="127"/>
+      <c r="K65" s="127"/>
+      <c r="L65" s="76"/>
+      <c r="M65" s="76"/>
+      <c r="N65" s="76"/>
+      <c r="O65" s="76"/>
+      <c r="P65" s="76"/>
+      <c r="Q65" s="76"/>
+      <c r="R65" s="76"/>
+    </row>
+    <row r="66" ht="48" customHeight="1" s="117" customFormat="1">
+      <c r="C66" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="D53" s="136" t="str">
+      <c r="D66" s="136" t="str">
         <f>'PROPOSAL'!F39</f>
         <v>EF - M-TU,TH-SU 03:00pm - 06:00pm, EF - M-SU 03:00pm - 06:00pm, EM - M-TU,TH-SU 06:00am - 09:00am, EM - M-SU 06:00am - 09:00am, MDN - M-TU,TH-SU 11:00am - 01:00pm, MDN - M-SU 11:00am - 01:00pm</v>
       </c>
-      <c r="E53" s="136"/>
-      <c r="F53" s="136"/>
-      <c r="G53" s="136"/>
-      <c r="H53" s="136"/>
-      <c r="I53" s="136"/>
-      <c r="J53" s="136"/>
-      <c r="K53" s="136"/>
-      <c r="L53" s="126"/>
-      <c r="M53" s="126"/>
-      <c r="N53" s="126"/>
-      <c r="O53" s="126"/>
-      <c r="P53" s="126"/>
-      <c r="Q53" s="126"/>
-      <c r="R53" s="126"/>
-    </row>
-    <row r="54" ht="8.1" customHeight="1" s="99" customFormat="1">
-      <c r="C54" s="2"/>
-      <c r="D54" s="128"/>
-      <c r="E54" s="128"/>
-      <c r="F54" s="128"/>
-      <c r="G54" s="128"/>
-      <c r="H54" s="128"/>
-      <c r="I54" s="128"/>
-      <c r="J54" s="128"/>
-      <c r="K54" s="128"/>
-      <c r="L54" s="118"/>
-      <c r="M54" s="118"/>
-      <c r="N54" s="118"/>
-      <c r="O54" s="118"/>
-      <c r="P54" s="118"/>
-      <c r="Q54" s="118"/>
-      <c r="R54" s="118"/>
-    </row>
-    <row r="55" ht="48" customHeight="1" s="99" customFormat="1">
-      <c r="C55" s="55" t="s">
+      <c r="E66" s="136"/>
+      <c r="F66" s="136"/>
+      <c r="G66" s="136"/>
+      <c r="H66" s="136"/>
+      <c r="I66" s="136"/>
+      <c r="J66" s="136"/>
+      <c r="K66" s="136"/>
+      <c r="L66" s="126"/>
+      <c r="M66" s="126"/>
+      <c r="N66" s="126"/>
+      <c r="O66" s="126"/>
+      <c r="P66" s="126"/>
+      <c r="Q66" s="126"/>
+      <c r="R66" s="126"/>
+    </row>
+    <row r="67" ht="8.1" customHeight="1" s="99" customFormat="1">
+      <c r="C67" s="2"/>
+      <c r="D67" s="128"/>
+      <c r="E67" s="128"/>
+      <c r="F67" s="128"/>
+      <c r="G67" s="128"/>
+      <c r="H67" s="128"/>
+      <c r="I67" s="128"/>
+      <c r="J67" s="128"/>
+      <c r="K67" s="128"/>
+      <c r="L67" s="118"/>
+      <c r="M67" s="118"/>
+      <c r="N67" s="118"/>
+      <c r="O67" s="118"/>
+      <c r="P67" s="118"/>
+      <c r="Q67" s="118"/>
+      <c r="R67" s="118"/>
+    </row>
+    <row r="68" ht="48" customHeight="1" s="99" customFormat="1">
+      <c r="C68" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="D55" s="136"/>
-      <c r="E55" s="136"/>
-      <c r="F55" s="136"/>
-      <c r="G55" s="136"/>
-      <c r="H55" s="136"/>
-      <c r="I55" s="136"/>
-      <c r="J55" s="136"/>
-      <c r="K55" s="136"/>
-      <c r="L55" s="126"/>
-      <c r="M55" s="126"/>
-      <c r="N55" s="126"/>
-      <c r="O55" s="126"/>
-      <c r="P55" s="126"/>
-      <c r="Q55" s="126"/>
-      <c r="R55" s="126"/>
-    </row>
-    <row r="56" ht="8.1" customHeight="1" s="99" customFormat="1">
-      <c r="C56" s="2"/>
-      <c r="D56" s="128"/>
-      <c r="E56" s="128"/>
-      <c r="F56" s="128"/>
-      <c r="G56" s="128"/>
-      <c r="H56" s="128"/>
-      <c r="I56" s="128"/>
-      <c r="J56" s="128"/>
-      <c r="K56" s="128"/>
-      <c r="L56" s="118"/>
-      <c r="M56" s="118"/>
-      <c r="N56" s="118"/>
-      <c r="O56" s="118"/>
-      <c r="P56" s="118"/>
-      <c r="Q56" s="118"/>
-      <c r="R56" s="118"/>
-    </row>
-    <row r="57" ht="48.95" customHeight="1" s="117" customFormat="1">
-      <c r="C57" s="55" t="s">
+      <c r="D68" s="136"/>
+      <c r="E68" s="136"/>
+      <c r="F68" s="136"/>
+      <c r="G68" s="136"/>
+      <c r="H68" s="136"/>
+      <c r="I68" s="136"/>
+      <c r="J68" s="136"/>
+      <c r="K68" s="136"/>
+      <c r="L68" s="126"/>
+      <c r="M68" s="126"/>
+      <c r="N68" s="126"/>
+      <c r="O68" s="126"/>
+      <c r="P68" s="126"/>
+      <c r="Q68" s="126"/>
+      <c r="R68" s="126"/>
+    </row>
+    <row r="69" ht="8.1" customHeight="1" s="99" customFormat="1">
+      <c r="C69" s="2"/>
+      <c r="D69" s="128"/>
+      <c r="E69" s="128"/>
+      <c r="F69" s="128"/>
+      <c r="G69" s="128"/>
+      <c r="H69" s="128"/>
+      <c r="I69" s="128"/>
+      <c r="J69" s="128"/>
+      <c r="K69" s="128"/>
+      <c r="L69" s="118"/>
+      <c r="M69" s="118"/>
+      <c r="N69" s="118"/>
+      <c r="O69" s="118"/>
+      <c r="P69" s="118"/>
+      <c r="Q69" s="118"/>
+      <c r="R69" s="118"/>
+    </row>
+    <row r="70" ht="48.95" customHeight="1" s="117" customFormat="1">
+      <c r="C70" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="D57" s="136" t="str">
+      <c r="D70" s="136" t="str">
         <f>'PROPOSAL'!F43</f>
         <v>3/19-3/20/20, 3/24/20, 3/28/20, 4/7/20, 4/9-3/17/20, 3/21/20, 3/26/20, 4/8-3/27/20, 3/29/20</v>
       </c>
-      <c r="E57" s="136"/>
-      <c r="F57" s="136"/>
-      <c r="G57" s="136"/>
-      <c r="H57" s="136"/>
-      <c r="I57" s="136"/>
-      <c r="J57" s="136"/>
-      <c r="K57" s="136"/>
-      <c r="L57" s="126"/>
-      <c r="M57" s="126"/>
-      <c r="N57" s="126"/>
-      <c r="O57" s="126"/>
-      <c r="P57" s="126"/>
-      <c r="Q57" s="126"/>
-      <c r="R57" s="126"/>
-    </row>
-    <row r="58" ht="8.1" customHeight="1" s="99" customFormat="1">
-      <c r="C58" s="2"/>
-      <c r="D58" s="128"/>
-      <c r="E58" s="128"/>
-      <c r="F58" s="128"/>
-      <c r="G58" s="128"/>
-      <c r="H58" s="128"/>
-      <c r="I58" s="128"/>
-      <c r="J58" s="128"/>
-      <c r="K58" s="128"/>
-      <c r="L58" s="118"/>
-      <c r="M58" s="118"/>
-      <c r="N58" s="118"/>
-      <c r="O58" s="118"/>
-      <c r="P58" s="118"/>
-      <c r="Q58" s="118"/>
-      <c r="R58" s="118"/>
-    </row>
-    <row r="59" ht="147" customHeight="1" s="99" customFormat="1">
-      <c r="C59" s="55" t="s">
+      <c r="E70" s="136"/>
+      <c r="F70" s="136"/>
+      <c r="G70" s="136"/>
+      <c r="H70" s="136"/>
+      <c r="I70" s="136"/>
+      <c r="J70" s="136"/>
+      <c r="K70" s="136"/>
+      <c r="L70" s="126"/>
+      <c r="M70" s="126"/>
+      <c r="N70" s="126"/>
+      <c r="O70" s="126"/>
+      <c r="P70" s="126"/>
+      <c r="Q70" s="126"/>
+      <c r="R70" s="126"/>
+    </row>
+    <row r="71" ht="8.1" customHeight="1" s="99" customFormat="1">
+      <c r="C71" s="2"/>
+      <c r="D71" s="128"/>
+      <c r="E71" s="128"/>
+      <c r="F71" s="128"/>
+      <c r="G71" s="128"/>
+      <c r="H71" s="128"/>
+      <c r="I71" s="128"/>
+      <c r="J71" s="128"/>
+      <c r="K71" s="128"/>
+      <c r="L71" s="118"/>
+      <c r="M71" s="118"/>
+      <c r="N71" s="118"/>
+      <c r="O71" s="118"/>
+      <c r="P71" s="118"/>
+      <c r="Q71" s="118"/>
+      <c r="R71" s="118"/>
+    </row>
+    <row r="72" ht="147" customHeight="1" s="99" customFormat="1">
+      <c r="C72" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="D59" s="136" t="str">
+      <c r="D72" s="136" t="str">
         <f>'PROPOSAL'!F45</f>
         <v>All CPMs are derived from 100% broadcast deliveries, no cable unless otherwise noted.</v>
       </c>
-      <c r="E59" s="136"/>
-      <c r="F59" s="136"/>
-      <c r="G59" s="136"/>
-      <c r="H59" s="136"/>
-      <c r="I59" s="136"/>
-      <c r="J59" s="136"/>
-      <c r="K59" s="136"/>
-      <c r="L59" s="77"/>
-      <c r="M59" s="77"/>
-      <c r="N59" s="77"/>
-      <c r="O59" s="77"/>
-      <c r="P59" s="77"/>
-      <c r="Q59" s="77"/>
-      <c r="R59" s="77"/>
-    </row>
-    <row r="60" ht="24" customHeight="1">
-      <c r="D60" s="135"/>
-      <c r="E60" s="135"/>
-      <c r="F60" s="135"/>
-      <c r="G60" s="135"/>
-      <c r="H60" s="135"/>
-      <c r="I60" s="135"/>
-      <c r="J60" s="135"/>
-      <c r="K60" s="135"/>
+      <c r="E72" s="136"/>
+      <c r="F72" s="136"/>
+      <c r="G72" s="136"/>
+      <c r="H72" s="136"/>
+      <c r="I72" s="136"/>
+      <c r="J72" s="136"/>
+      <c r="K72" s="136"/>
+      <c r="L72" s="77"/>
+      <c r="M72" s="77"/>
+      <c r="N72" s="77"/>
+      <c r="O72" s="77"/>
+      <c r="P72" s="77"/>
+      <c r="Q72" s="77"/>
+      <c r="R72" s="77"/>
+    </row>
+    <row r="73" ht="24" customHeight="1">
+      <c r="D73" s="135"/>
+      <c r="E73" s="135"/>
+      <c r="F73" s="135"/>
+      <c r="G73" s="135"/>
+      <c r="H73" s="135"/>
+      <c r="I73" s="135"/>
+      <c r="J73" s="135"/>
+      <c r="K73" s="135"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="D60:K60"/>
-    <mergeCell ref="D59:K59"/>
-    <mergeCell ref="D51:K51"/>
-    <mergeCell ref="D53:K53"/>
-    <mergeCell ref="D55:K55"/>
-    <mergeCell ref="D57:K57"/>
+    <mergeCell ref="D73:K73"/>
+    <mergeCell ref="D72:K72"/>
+    <mergeCell ref="D64:K64"/>
+    <mergeCell ref="D66:K66"/>
+    <mergeCell ref="D68:K68"/>
+    <mergeCell ref="D70:K70"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:K1048576">
     <cfRule type="expression" dxfId="0" priority="5">
@@ -13210,97 +13527,97 @@
     <row r="1" ht="18" customHeight="1"/>
     <row r="2" ht="27.95" customHeight="1">
       <c r="D2" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
     <row r="4" ht="104.1" customHeight="1" s="116" customFormat="1">
       <c r="C4" s="144" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D4" s="144"/>
     </row>
     <row r="5" ht="110.1" customHeight="1" s="116" customFormat="1">
       <c r="C5" s="144" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D5" s="144"/>
     </row>
     <row r="6" ht="209.1" customHeight="1" s="116" customFormat="1">
       <c r="C6" s="144" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D6" s="144"/>
     </row>
     <row r="7" ht="89.1" customHeight="1" s="116" customFormat="1">
       <c r="C7" s="144" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D7" s="144"/>
     </row>
     <row r="8" ht="150" customHeight="1" s="116" customFormat="1">
       <c r="C8" s="144" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D8" s="144"/>
     </row>
     <row r="9" ht="200.1" customHeight="1" s="116" customFormat="1">
       <c r="C9" s="144" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D9" s="144"/>
     </row>
     <row r="10" ht="147.95" customHeight="1" s="116" customFormat="1">
       <c r="C10" s="144" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D10" s="144"/>
     </row>
     <row r="11" ht="134.1" customHeight="1" s="116" customFormat="1">
       <c r="C11" s="144" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D11" s="144"/>
     </row>
     <row r="12" ht="54" customHeight="1" s="116" customFormat="1">
       <c r="C12" s="144" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D12" s="144"/>
     </row>
     <row r="13" ht="69.95" customHeight="1" s="116" customFormat="1">
       <c r="C13" s="144" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D13" s="144"/>
     </row>
     <row r="14" ht="128.1" customHeight="1" s="116" customFormat="1">
       <c r="C14" s="144" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D14" s="144"/>
     </row>
     <row r="15" ht="51.95" customHeight="1" s="116" customFormat="1">
       <c r="C15" s="144" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D15" s="144"/>
     </row>
     <row r="16" ht="84" customHeight="1" s="116" customFormat="1">
       <c r="C16" s="144" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D16" s="144"/>
     </row>
     <row r="17" ht="69.95" customHeight="1" s="116" customFormat="1">
       <c r="C17" s="144" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D17" s="144"/>
     </row>
     <row r="18" ht="180" customHeight="1" s="116" customFormat="1">
       <c r="C18" s="144" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D18" s="144"/>
     </row>
@@ -13361,10 +13678,10 @@
     <row r="2" ht="27.95" customHeight="1">
       <c r="E2" s="5"/>
       <c r="F2" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -13399,24 +13716,24 @@
     </row>
     <row r="5" ht="18" customHeight="1" s="3" customFormat="1">
       <c r="C5" s="134" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D5" s="134"/>
       <c r="E5" s="134" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F5" s="134"/>
       <c r="G5" s="134"/>
       <c r="H5" s="134" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I5" s="134"/>
       <c r="J5" s="134" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K5" s="134"/>
       <c r="L5" s="134" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M5" s="134"/>
       <c r="N5" s="76" t="s">
@@ -13428,7 +13745,7 @@
       <c r="R5" s="134"/>
       <c r="S5" s="134"/>
       <c r="T5" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" ht="18" customHeight="1">
@@ -13463,7 +13780,7 @@
       <c r="L7" s="139"/>
       <c r="M7" s="140"/>
       <c r="N7" s="138" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="O7" s="139"/>
       <c r="P7" s="139"/>
@@ -13481,7 +13798,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E8" s="40" t="s">
         <v>23</v>
@@ -13541,7 +13858,7 @@
         <v>104</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="E9" s="119">
         <v>0</v>
@@ -13598,10 +13915,10 @@
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="E10" s="119">
         <v>0</v>
@@ -13658,10 +13975,10 @@
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="E11" s="119">
         <v>0</v>
@@ -13718,7 +14035,7 @@
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>147</v>
@@ -13838,7 +14155,7 @@
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>147</v>
@@ -13949,7 +14266,7 @@
     </row>
     <row r="17" ht="24" customHeight="1">
       <c r="C17" s="53" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D17" s="53"/>
       <c r="E17" s="7"/>
@@ -13964,7 +14281,7 @@
       <c r="L17" s="139"/>
       <c r="M17" s="140"/>
       <c r="N17" s="138" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="O17" s="139"/>
       <c r="P17" s="139"/>
@@ -13982,7 +14299,7 @@
         <v>22</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E18" s="40" t="s">
         <v>23</v>
@@ -14042,7 +14359,7 @@
         <v>104</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="E19" s="119">
         <v>0</v>
@@ -14099,10 +14416,10 @@
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="E20" s="119">
         <v>0</v>
@@ -14159,10 +14476,10 @@
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="E21" s="119">
         <v>0</v>
@@ -14219,7 +14536,7 @@
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>147</v>
@@ -14339,7 +14656,7 @@
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>147</v>
@@ -14465,7 +14782,7 @@
       <c r="L27" s="139"/>
       <c r="M27" s="140"/>
       <c r="N27" s="138" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="O27" s="139"/>
       <c r="P27" s="139"/>
@@ -14483,7 +14800,7 @@
         <v>22</v>
       </c>
       <c r="D28" s="40" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E28" s="40" t="s">
         <v>23</v>
@@ -14543,7 +14860,7 @@
         <v>104</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="E29" s="119">
         <v>0</v>
@@ -14600,10 +14917,10 @@
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="E30" s="119">
         <v>0</v>
@@ -14660,10 +14977,10 @@
       </c>
       <c r="B31" s="25"/>
       <c r="C31" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="E31" s="119">
         <v>0</v>
@@ -14720,7 +15037,7 @@
       </c>
       <c r="B32" s="25"/>
       <c r="C32" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>147</v>
@@ -14840,7 +15157,7 @@
       </c>
       <c r="B34" s="25"/>
       <c r="C34" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>147</v>

</xml_diff>

<commit_message>
Merged PR 7604: PRI-22222 Proposal tab - Secondary Audiences - Campaign Totals
PRI-22222 Implementation and tests
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
@@ -829,7 +829,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 02/25/20</t>
+    <t>Created 02/26/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -1310,7 +1310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="145">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="8" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="1"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
@@ -1741,9 +1741,6 @@
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="10" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2486,7 +2483,7 @@
       </c>
       <c r="L2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 02/25/20</v>
+        <v>Created 02/26/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -4397,7 +4394,7 @@
       <c r="K2" s="5"/>
       <c r="P2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 02/25/20</v>
+        <v>Created 02/26/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -14860,8 +14857,8 @@
       <c r="E29" s="119">
         <v>0</v>
       </c>
-      <c r="F29" s="120" t="s">
-        <v>38</v>
+      <c r="F29" s="120">
+        <v>0</v>
       </c>
       <c r="G29" s="121">
         <v>200000</v>
@@ -14920,8 +14917,8 @@
       <c r="E30" s="119">
         <v>0</v>
       </c>
-      <c r="F30" s="120" t="s">
-        <v>38</v>
+      <c r="F30" s="120">
+        <v>0</v>
       </c>
       <c r="G30" s="121">
         <v>200000</v>
@@ -14980,8 +14977,8 @@
       <c r="E31" s="119">
         <v>0</v>
       </c>
-      <c r="F31" s="120" t="s">
-        <v>38</v>
+      <c r="F31" s="120">
+        <v>0</v>
       </c>
       <c r="G31" s="121">
         <v>100000</v>
@@ -15040,8 +15037,8 @@
       <c r="E32" s="119">
         <v>0</v>
       </c>
-      <c r="F32" s="120" t="s">
-        <v>38</v>
+      <c r="F32" s="120">
+        <v>0</v>
       </c>
       <c r="G32" s="121">
         <v>1000</v>
@@ -15100,8 +15097,8 @@
       <c r="E33" s="119">
         <v>0</v>
       </c>
-      <c r="F33" s="120" t="s">
-        <v>38</v>
+      <c r="F33" s="120">
+        <v>0</v>
       </c>
       <c r="G33" s="121">
         <v>2000</v>
@@ -15160,8 +15157,8 @@
       <c r="E34" s="119">
         <v>0</v>
       </c>
-      <c r="F34" s="120" t="s">
-        <v>38</v>
+      <c r="F34" s="120">
+        <v>0</v>
       </c>
       <c r="G34" s="121">
         <v>497000</v>
@@ -15261,196 +15258,62 @@
         <v>3345.69</v>
       </c>
     </row>
-    <row r="37" ht="48" customHeight="1">
+    <row r="36" ht="8.1" customHeight="1">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="F36" s="118"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="118"/>
+      <c r="I36" s="118"/>
+      <c r="J36" s="118"/>
+      <c r="K36" s="118"/>
+      <c r="L36" s="118"/>
+      <c r="M36" s="118"/>
+      <c r="N36" s="118"/>
+      <c r="O36" s="118"/>
+      <c r="P36" s="118"/>
+      <c r="Q36" s="118"/>
+      <c r="R36" s="118"/>
+      <c r="S36" s="118"/>
+      <c r="T36" s="118"/>
+    </row>
+    <row r="37" ht="147" customHeight="1">
       <c r="C37" s="55" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D37" s="55"/>
-      <c r="E37" s="117"/>
-      <c r="F37" s="145" t="s">
+      <c r="F37" s="136" t="s">
         <v>123</v>
       </c>
-      <c r="G37" s="145"/>
-      <c r="H37" s="145"/>
-      <c r="I37" s="145"/>
-      <c r="J37" s="145"/>
-      <c r="K37" s="145"/>
-      <c r="L37" s="145"/>
-      <c r="M37" s="145"/>
-      <c r="N37" s="145"/>
-      <c r="O37" s="145"/>
-      <c r="P37" s="145"/>
-      <c r="Q37" s="145"/>
-      <c r="R37" s="145"/>
-      <c r="S37" s="145"/>
-      <c r="T37" s="145"/>
-    </row>
-    <row r="38" ht="8.1" customHeight="1">
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="76"/>
-      <c r="H38" s="76"/>
-      <c r="I38" s="76"/>
-      <c r="J38" s="76"/>
-      <c r="K38" s="76"/>
-      <c r="L38" s="76"/>
-      <c r="M38" s="76"/>
-      <c r="N38" s="76"/>
-      <c r="O38" s="76"/>
-      <c r="P38" s="76"/>
-      <c r="Q38" s="76"/>
-      <c r="R38" s="76"/>
-      <c r="S38" s="76"/>
-      <c r="T38" s="76"/>
-    </row>
-    <row r="39" ht="48" customHeight="1" s="117" customFormat="1">
-      <c r="C39" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="55"/>
-      <c r="F39" s="145" t="s">
+      <c r="G37" s="136"/>
+      <c r="H37" s="136"/>
+      <c r="I37" s="136"/>
+      <c r="J37" s="136"/>
+      <c r="K37" s="136"/>
+      <c r="L37" s="136"/>
+      <c r="M37" s="136"/>
+      <c r="N37" s="136"/>
+      <c r="O37" s="136"/>
+      <c r="P37" s="136"/>
+      <c r="Q37" s="136"/>
+      <c r="R37" s="136"/>
+      <c r="S37" s="136"/>
+      <c r="T37" s="136"/>
+    </row>
+    <row r="39">
+      <c r="F39" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="G39" s="145"/>
-      <c r="H39" s="145"/>
-      <c r="I39" s="145"/>
-      <c r="J39" s="145"/>
-      <c r="K39" s="145"/>
-      <c r="L39" s="145"/>
-      <c r="M39" s="145"/>
-      <c r="N39" s="145"/>
-      <c r="O39" s="145"/>
-      <c r="P39" s="145"/>
-      <c r="Q39" s="145"/>
-      <c r="R39" s="145"/>
-      <c r="S39" s="145"/>
-      <c r="T39" s="145"/>
-    </row>
-    <row r="40" ht="8.1" customHeight="1">
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="F40" s="118"/>
-      <c r="G40" s="118"/>
-      <c r="H40" s="118"/>
-      <c r="I40" s="118"/>
-      <c r="J40" s="118"/>
-      <c r="K40" s="118"/>
-      <c r="L40" s="118"/>
-      <c r="M40" s="118"/>
-      <c r="N40" s="118"/>
-      <c r="O40" s="118"/>
-      <c r="P40" s="118"/>
-      <c r="Q40" s="118"/>
-      <c r="R40" s="118"/>
-      <c r="S40" s="118"/>
-      <c r="T40" s="118"/>
-    </row>
-    <row r="41" ht="48" customHeight="1">
-      <c r="C41" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="55"/>
-      <c r="E41" s="117"/>
-      <c r="F41" s="145"/>
-      <c r="G41" s="145"/>
-      <c r="H41" s="145"/>
-      <c r="I41" s="145"/>
-      <c r="J41" s="145"/>
-      <c r="K41" s="145"/>
-      <c r="L41" s="145"/>
-      <c r="M41" s="145"/>
-      <c r="N41" s="145"/>
-      <c r="O41" s="145"/>
-      <c r="P41" s="145"/>
-      <c r="Q41" s="145"/>
-      <c r="R41" s="145"/>
-      <c r="S41" s="145"/>
-      <c r="T41" s="145"/>
-    </row>
-    <row r="42" ht="8.1" customHeight="1">
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="F42" s="118"/>
-      <c r="G42" s="118"/>
-      <c r="H42" s="118"/>
-      <c r="I42" s="118"/>
-      <c r="J42" s="118"/>
-      <c r="K42" s="118"/>
-      <c r="L42" s="118"/>
-      <c r="M42" s="118"/>
-      <c r="N42" s="118"/>
-      <c r="O42" s="118"/>
-      <c r="P42" s="118"/>
-      <c r="Q42" s="118"/>
-      <c r="R42" s="118"/>
-      <c r="S42" s="118"/>
-      <c r="T42" s="118"/>
-    </row>
-    <row r="43" ht="48.95" customHeight="1" s="117" customFormat="1">
-      <c r="C43" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="D43" s="55"/>
-      <c r="F43" s="145" t="s">
+    </row>
+    <row r="43">
+      <c r="F43" s="99" t="s">
         <v>124</v>
       </c>
-      <c r="G43" s="145"/>
-      <c r="H43" s="145"/>
-      <c r="I43" s="145"/>
-      <c r="J43" s="145"/>
-      <c r="K43" s="145"/>
-      <c r="L43" s="145"/>
-      <c r="M43" s="145"/>
-      <c r="N43" s="145"/>
-      <c r="O43" s="145"/>
-      <c r="P43" s="145"/>
-      <c r="Q43" s="145"/>
-      <c r="R43" s="145"/>
-      <c r="S43" s="145"/>
-      <c r="T43" s="145"/>
-    </row>
-    <row r="44" ht="8.1" customHeight="1">
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="F44" s="118"/>
-      <c r="G44" s="118"/>
-      <c r="H44" s="118"/>
-      <c r="I44" s="118"/>
-      <c r="J44" s="118"/>
-      <c r="K44" s="118"/>
-      <c r="L44" s="118"/>
-      <c r="M44" s="118"/>
-      <c r="N44" s="118"/>
-      <c r="O44" s="118"/>
-      <c r="P44" s="118"/>
-      <c r="Q44" s="118"/>
-      <c r="R44" s="118"/>
-      <c r="S44" s="118"/>
-      <c r="T44" s="118"/>
-    </row>
-    <row r="45" ht="147" customHeight="1">
-      <c r="C45" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="55"/>
-      <c r="F45" s="136" t="s">
+    </row>
+    <row r="45">
+      <c r="F45" s="99" t="s">
         <v>125</v>
       </c>
-      <c r="G45" s="136"/>
-      <c r="H45" s="136"/>
-      <c r="I45" s="136"/>
-      <c r="J45" s="136"/>
-      <c r="K45" s="136"/>
-      <c r="L45" s="136"/>
-      <c r="M45" s="136"/>
-      <c r="N45" s="136"/>
-      <c r="O45" s="136"/>
-      <c r="P45" s="136"/>
-      <c r="Q45" s="136"/>
-      <c r="R45" s="136"/>
-      <c r="S45" s="136"/>
-      <c r="T45" s="136"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -15458,16 +15321,12 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
-    <mergeCell ref="F39:T39"/>
-    <mergeCell ref="F41:T41"/>
-    <mergeCell ref="F43:T43"/>
-    <mergeCell ref="F45:T45"/>
+    <mergeCell ref="F37:T37"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="Q5:S5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H7:M7"/>
     <mergeCell ref="N7:T7"/>
-    <mergeCell ref="F37:T37"/>
     <mergeCell ref="H17:M17"/>
     <mergeCell ref="N17:T17"/>
     <mergeCell ref="H27:M27"/>

</xml_diff>

<commit_message>
Merged PR 7641: PRI-23210 Quarterly totals ADU table-Aggregated hiatus days are not displayed
PRI-23210 Bug fix and tests
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
@@ -829,7 +829,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 02/27/20</t>
+    <t>Created 02/29/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="L2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 02/27/20</v>
+        <v>Created 02/29/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -4334,7 +4334,7 @@
       <c r="K2" s="5"/>
       <c r="P2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 02/27/20</v>
+        <v>Created 02/29/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -7572,10 +7572,18 @@
       <c r="J95" s="133"/>
       <c r="K95" s="131"/>
       <c r="L95" s="132"/>
-      <c r="M95" s="132"/>
-      <c r="N95" s="132"/>
-      <c r="O95" s="133"/>
-      <c r="P95" s="130"/>
+      <c r="M95" s="132" t="s">
+        <v>62</v>
+      </c>
+      <c r="N95" s="132" t="s">
+        <v>69</v>
+      </c>
+      <c r="O95" s="133" t="s">
+        <v>70</v>
+      </c>
+      <c r="P95" s="130">
+        <v>11</v>
+      </c>
     </row>
     <row r="97">
       <c r="B97" s="53" t="s">
@@ -10725,7 +10733,9 @@
         <v>61</v>
       </c>
       <c r="C185" s="131"/>
-      <c r="D185" s="132"/>
+      <c r="D185" s="132" t="s">
+        <v>87</v>
+      </c>
       <c r="E185" s="132"/>
       <c r="F185" s="132"/>
       <c r="G185" s="131"/>
@@ -10737,7 +10747,9 @@
       <c r="M185" s="132"/>
       <c r="N185" s="132"/>
       <c r="O185" s="133"/>
-      <c r="P185" s="130"/>
+      <c r="P185" s="130">
+        <v>5</v>
+      </c>
     </row>
     <row r="188" ht="24" customHeight="1">
       <c r="P188" s="60"/>

</xml_diff>

<commit_message>
Merged PR 7669: PRI-23500 Total GRPs value is displayed on a different column in the Quarterly & Campaigns total table when Secondary Audience is selected
PRI-23500 Bug fix and tests
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
@@ -829,7 +829,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 02/29/20</t>
+    <t>Created 03/02/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="L2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 02/29/20</v>
+        <v>Created 03/02/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -4334,7 +4334,7 @@
       <c r="K2" s="5"/>
       <c r="P2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 02/29/20</v>
+        <v>Created 03/02/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>

</xml_diff>

<commit_message>
Merged PR 7687: PRI-23333 Do Not Allow Export of Multiple Plans with different Secondary Audiences
PRI-23333 Implementation and tests
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
@@ -829,7 +829,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 03/02/20</t>
+    <t>Created 03/03/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="L2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 03/02/20</v>
+        <v>Created 03/03/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -4334,7 +4334,7 @@
       <c r="K2" s="5"/>
       <c r="P2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 03/02/20</v>
+        <v>Created 03/03/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>

</xml_diff>

<commit_message>
Merged PR 7721: PRI-23754 Proposal tab- Flight Hiatuses- incorrect date ranges displayed for individual days
PRI-23754 Bug fix and tests
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
@@ -408,7 +408,7 @@
     <t>~80% Minimum TV HH Coverage | Blackout Markets: Lansing, Wilmington, Presque Isle | Preferential Markets: Philadelphia, Macon, New York, Binghamton</t>
   </si>
   <si>
-    <t>3/19-3/20/20, 3/24/20, 3/28/20, 4/7/20, 4/9-3/17/20, 3/21/20, 3/26/20, 4/8-3/27/20, 3/29/20</t>
+    <t>3/15-3/17/20, 3/19-3/21/20, 3/24/20, 3/26-3/29/20, 4/7-4/11/20</t>
   </si>
   <si>
     <t>All CPMs are derived from 100% broadcast deliveries, no cable unless otherwise noted.</t>
@@ -829,7 +829,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 03/03/20</t>
+    <t>Created 03/05/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="L2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 03/03/20</v>
+        <v>Created 03/05/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -4334,7 +4334,7 @@
       <c r="K2" s="5"/>
       <c r="P2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 03/03/20</v>
+        <v>Created 03/05/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>

</xml_diff>

<commit_message>
Merged PR 7785: PRI-23922 Quarter & totals table- Discrepancy between the Report & UI -Weekly Impression and Cost
PRI-23922 Bug fix
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
@@ -829,7 +829,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 03/05/20</t>
+    <t>Created 03/10/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="L2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 03/05/20</v>
+        <v>Created 03/10/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -4334,7 +4334,7 @@
       <c r="K2" s="5"/>
       <c r="P2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 03/05/20</v>
+        <v>Created 03/10/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>

</xml_diff>

<commit_message>
Merged PR 7827: PRI-24059 Quarterly & totals table- Incorrect Total impressions, CPP, & Cost populated
PRI-24059 Implementation and tests
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractOnlyPlans.xlsx
@@ -829,7 +829,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 03/10/20</t>
+    <t>Created 03/12/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -2423,7 +2423,7 @@
       </c>
       <c r="L2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 03/10/20</v>
+        <v>Created 03/12/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -4334,7 +4334,7 @@
       <c r="K2" s="5"/>
       <c r="P2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 03/10/20</v>
+        <v>Created 03/12/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>

</xml_diff>